<commit_message>
analisis del site 2.0
</commit_message>
<xml_diff>
--- a/Analisis QA del site.xlsx
+++ b/Analisis QA del site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="14640" windowHeight="5085"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="14640" windowHeight="5085"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>COSAS EXTERNAS</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Exportar reportes a excel</t>
   </si>
   <si>
-    <t>agregar campo "Ciudad" en abm de usuario</t>
-  </si>
-  <si>
     <t>cambiar el apellido del dogor en "acerca de" por casuscelli</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>agregar fotito del emprendimiento a la izquierda</t>
   </si>
   <si>
-    <t xml:space="preserve">Que funcione el buscador </t>
-  </si>
-  <si>
     <t>/confirmarPago</t>
   </si>
   <si>
@@ -207,13 +201,56 @@
   </si>
   <si>
     <t>configurar parameters.yml de gmail para que salgan los mails</t>
+  </si>
+  <si>
+    <t>Separar las notificaciones con espacios o lineas, y ponerle la fecha del comentario</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">agregar campo "Ciudad" en abm de usuario. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>¿PARA QUE ERA ESTO?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Que funcione el buscador </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>SE ROMPE AL BUSCAR</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,8 +294,22 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +319,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +377,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,11 +661,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D82"/>
+  <dimension ref="B1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -630,31 +701,31 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="7"/>
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="7"/>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -665,311 +736,318 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="7"/>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="7"/>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="7"/>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="4"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="4"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="7"/>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="7"/>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="4"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="7"/>
       <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="9"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D36" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="4"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="7"/>
       <c r="D38" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="4"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="1" t="s">
-        <v>21</v>
+      <c r="D39" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="4"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="1" t="s">
-        <v>22</v>
+      <c r="D40" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D43" s="3" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="8"/>
+      <c r="D45" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="8"/>
+      <c r="D46" s="11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="4"/>
-      <c r="D44" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
-      <c r="D45" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="4"/>
-      <c r="D46" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="D47" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
       <c r="D48" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+      <c r="D49" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="10"/>
+      <c r="D52" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="4"/>
-      <c r="D51" s="1" t="s">
+    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="10"/>
+      <c r="D55" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="4"/>
-      <c r="D54" s="1" t="s">
+    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="4"/>
+      <c r="D58" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="10"/>
+      <c r="D61" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="4"/>
-      <c r="D57" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="4"/>
-      <c r="D60" s="1" t="s">
+    <row r="63" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D62" s="2" t="s">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="10"/>
+      <c r="D64" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="4"/>
-      <c r="D63" s="1" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="8"/>
+      <c r="D65" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B64" s="4"/>
-      <c r="D64" s="1" t="s">
+    <row r="67" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B68" s="8"/>
+      <c r="D68" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B69" s="8"/>
+      <c r="D69" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D66" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="4"/>
-      <c r="D67" s="1" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="8"/>
+      <c r="D72" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="4"/>
-      <c r="D68" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="D73" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="4"/>
-      <c r="D71" s="1" t="s">
+    <row r="75" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="D75" s="6" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B72" s="4"/>
-      <c r="D72" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="D74" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B76" s="4"/>
-      <c r="D76" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="4"/>
       <c r="D77" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="D79" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="4"/>
-      <c r="D81" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B78" s="4"/>
+      <c r="D78" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="D80" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="4"/>
       <c r="D82" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="D83" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analisis QA del site v3
</commit_message>
<xml_diff>
--- a/Analisis QA del site.xlsx
+++ b/Analisis QA del site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="14640" windowHeight="5085"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="14640" windowHeight="5085"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>COSAS EXTERNAS</t>
   </si>
@@ -245,12 +245,30 @@
       <t>SE ROMPE AL BUSCAR</t>
     </r>
   </si>
+  <si>
+    <t>Arreglar el formulario de emprendedor</t>
+  </si>
+  <si>
+    <t>agregar datos de telefono, mail y direccion al listado de emprendedores pendientes</t>
+  </si>
+  <si>
+    <t>poner logo de mercado pago</t>
+  </si>
+  <si>
+    <t>que el listado de inversiones se muestre dos segundos despues de dejar posicionado el mouse</t>
+  </si>
+  <si>
+    <t>cambiar texto "Se notificado correctamente" por "se ha notificado correctamente"</t>
+  </si>
+  <si>
+    <t>hacer tabla de historial de ganancias general. Si permite seleccionar la data y copiarla mejor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +326,15 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +362,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -381,6 +412,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,9 +696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D83"/>
+  <dimension ref="B1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -763,290 +800,332 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
-        <v>10</v>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
+      <c r="D21" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="7"/>
       <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="D27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="7"/>
       <c r="D30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="10"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="4"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D33" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="10"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="7"/>
       <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="9"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D37" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="10"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="7"/>
       <c r="D38" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="8"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="8"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="11" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="8"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="7"/>
       <c r="D41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="8"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="8"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="10"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="1" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="10"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D44" s="3" t="s">
+    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="8"/>
-      <c r="D45" s="1" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="8"/>
+      <c r="D48" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="8"/>
-      <c r="D46" s="11" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="8"/>
+      <c r="D49" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="4"/>
-      <c r="D47" s="1" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="4"/>
+      <c r="D50" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="4"/>
-      <c r="D48" s="1" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
+      <c r="D51" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="10"/>
-      <c r="D49" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="D52" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="10"/>
       <c r="D55" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="4"/>
+      <c r="B58" s="10"/>
       <c r="D58" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="10"/>
+      <c r="B61" s="4"/>
       <c r="D61" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
       <c r="D64" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="8"/>
       <c r="D65" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" s="12"/>
     </row>
     <row r="67" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="8"/>
-      <c r="D68" s="11" t="s">
-        <v>61</v>
+      <c r="B68" s="10"/>
+      <c r="D68" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" s="8"/>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B70" s="14"/>
+      <c r="D70" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="15"/>
+      <c r="D71" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="8"/>
+      <c r="D73" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" s="8"/>
+      <c r="D74" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+    <row r="76" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B72" s="8"/>
-      <c r="D72" s="11" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B77" s="8"/>
+      <c r="D77" s="11" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="4"/>
-      <c r="D73" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="D75" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B77" s="4"/>
-      <c r="D77" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="4"/>
       <c r="D78" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D80" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="4"/>
       <c r="D82" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="4"/>
       <c r="D83" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="D85" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="D87" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88" s="4"/>
+      <c r="D88" s="1" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>